<commit_message>
Mert'in 10.000 ruble avansı var; Ağustos maaşına devredecek
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/TEMMUZ 2025/2025 TEMMUZ AYI - TURKLER.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/TEMMUZ 2025/2025 TEMMUZ AYI - TURKLER.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">2025 TEMMUZ AYI TURKLER</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">DEMIRAYAK MERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.000 RUBLE AVANSTA</t>
   </si>
   <si>
     <t xml:space="preserve">CELIK HASAN</t>
@@ -404,40 +407,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,31 +452,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,51 +484,55 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,27 +540,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -746,502 +757,505 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="n">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="n">
         <v>2500</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="10" t="n">
         <f aca="false">F3*K3</f>
         <v>202500</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="n">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="n">
         <f aca="false">G3-H3</f>
         <v>202500</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11" t="n">
+      <c r="J3" s="11"/>
+      <c r="K3" s="12" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+      <c r="A4" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="n">
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="n">
         <v>2500</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="18" t="n">
         <f aca="false">F4*K4</f>
         <v>202500</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17" t="n">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="n">
         <f aca="false">G4-H4</f>
         <v>202500</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19" t="n">
+      <c r="J4" s="19"/>
+      <c r="K4" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="16" t="n">
         <v>357</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F5" s="16" t="n">
+      <c r="F5" s="17" t="n">
         <f aca="false">D5*E5</f>
         <v>2499</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="18" t="n">
         <f aca="false">F5*K5</f>
         <v>202419</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17" t="n">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="n">
         <f aca="false">G5-H5</f>
         <v>202419</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19" t="n">
+      <c r="J5" s="19"/>
+      <c r="K5" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="16" t="n">
         <v>377</v>
       </c>
-      <c r="E6" s="16" t="n">
+      <c r="E6" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F6" s="16" t="n">
+      <c r="F6" s="17" t="n">
         <f aca="false">D6*E6</f>
         <v>2639</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="18" t="n">
         <f aca="false">F6*K6</f>
         <v>213759</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17" t="n">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="n">
         <f aca="false">G6-H6</f>
         <v>213759</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19" t="n">
+      <c r="J6" s="19"/>
+      <c r="K6" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
+      <c r="A7" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16" t="n">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="F7" s="16" t="n">
+      <c r="F7" s="17" t="n">
         <f aca="false">D7*E7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="18" t="n">
         <f aca="false">F7*K7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17" t="n">
+      <c r="H7" s="18"/>
+      <c r="I7" s="18" t="n">
         <f aca="false">G7-H7</f>
         <v>0</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19" t="n">
+      <c r="J7" s="19"/>
+      <c r="K7" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="n">
+      <c r="A8" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="16" t="n">
         <v>380</v>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F8" s="16" t="n">
+      <c r="F8" s="17" t="n">
         <f aca="false">D8*E8</f>
         <v>2660</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="18" t="n">
         <f aca="false">F8*K8</f>
         <v>215460</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17" t="n">
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="n">
         <f aca="false">G8-H8</f>
         <v>215460</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19" t="n">
+      <c r="J8" s="19"/>
+      <c r="K8" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
+      <c r="A9" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="16" t="n">
         <v>377</v>
       </c>
-      <c r="E9" s="16" t="n">
+      <c r="E9" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F9" s="16" t="n">
+      <c r="F9" s="17" t="n">
         <f aca="false">D9*E9</f>
         <v>2639</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="18" t="n">
         <f aca="false">F9*K9</f>
         <v>213759</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17" t="n">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18" t="n">
         <f aca="false">G9-H9</f>
         <v>213759</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19" t="n">
+      <c r="J9" s="19"/>
+      <c r="K9" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
+      <c r="A10" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="n">
+      <c r="B10" s="14" t="n">
         <v>263</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16" t="n">
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="n">
         <v>2000</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="18" t="n">
         <f aca="false">F10*K10</f>
         <v>162000</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17" t="n">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="n">
         <f aca="false">G10-H10</f>
         <v>162000</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19" t="n">
+      <c r="J10" s="19"/>
+      <c r="K10" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
+      <c r="A11" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="n">
+      <c r="B11" s="14" t="n">
         <v>282</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="15" t="n">
+      <c r="D11" s="16" t="n">
         <v>346</v>
       </c>
-      <c r="E11" s="16" t="n">
+      <c r="E11" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F11" s="16" t="n">
+      <c r="F11" s="17" t="n">
         <f aca="false">D11*E11</f>
         <v>2422</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="18" t="n">
         <f aca="false">F11*K11</f>
         <v>196182</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17" t="n">
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="n">
         <f aca="false">G11-H11</f>
         <v>196182</v>
       </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19" t="n">
+      <c r="J11" s="19"/>
+      <c r="K11" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="n">
+      <c r="A12" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="n">
+      <c r="B12" s="14" t="n">
         <v>283</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="15" t="n">
+      <c r="D12" s="16" t="n">
         <v>262</v>
       </c>
-      <c r="E12" s="16" t="n">
+      <c r="E12" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F12" s="16" t="n">
+      <c r="F12" s="17" t="n">
         <f aca="false">D12*E12</f>
         <v>1834</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="18" t="n">
         <f aca="false">F12*K12</f>
         <v>148554</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17" t="n">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="n">
         <f aca="false">G12-H12</f>
         <v>148554</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19" t="n">
+      <c r="J12" s="19"/>
+      <c r="K12" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="n">
+      <c r="A13" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="n">
+      <c r="B13" s="14" t="n">
         <v>360</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="16" t="n">
         <v>317</v>
       </c>
-      <c r="E13" s="16" t="n">
+      <c r="E13" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="F13" s="16" t="n">
+      <c r="F13" s="17" t="n">
         <f aca="false">D13*E13</f>
         <v>1902</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="18" t="n">
         <f aca="false">F13*K13</f>
         <v>154062</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17" t="n">
+      <c r="H13" s="18"/>
+      <c r="I13" s="18" t="n">
         <f aca="false">G13-H13</f>
         <v>154062</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19" t="n">
+      <c r="J13" s="19"/>
+      <c r="K13" s="20" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="n">
+      <c r="A14" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="n">
+      <c r="B14" s="14" t="n">
         <v>387</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="16" t="n">
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="18" t="n">
         <f aca="false">F14*K14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17" t="n">
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="n">
         <f aca="false">G14-H14</f>
         <v>0</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="19" t="n">
+      <c r="J14" s="24"/>
+      <c r="K14" s="20" t="n">
         <v>81</v>
       </c>
+      <c r="L14" s="25" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="n">
+      <c r="A15" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="25" t="n">
+      <c r="B15" s="27" t="n">
         <v>399</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29" t="n">
+      <c r="C15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="n">
         <v>2000</v>
       </c>
-      <c r="G15" s="30" t="n">
+      <c r="G15" s="32" t="n">
         <f aca="false">F15*K15</f>
         <v>162000</v>
       </c>
-      <c r="H15" s="30" t="n">
+      <c r="H15" s="32" t="n">
         <v>162000</v>
       </c>
-      <c r="I15" s="30" t="n">
+      <c r="I15" s="32" t="n">
         <f aca="false">G15-H15</f>
         <v>0</v>
       </c>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32" t="n">
+      <c r="J15" s="33"/>
+      <c r="K15" s="34" t="n">
         <v>81</v>
       </c>
-      <c r="L15" s="33" t="s">
-        <v>32</v>
+      <c r="L15" s="35" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="34" t="n">
+      <c r="F17" s="36" t="n">
         <f aca="false">SUM(F3:F16)</f>
         <v>25595</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="36" t="n">
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38" t="n">
         <f aca="false">SUM(I3:I16)</f>
         <v>1911195</v>
       </c>

</xml_diff>